<commit_message>
Add new Excel files for Auto Optuna ML search results
- Created S01_search_2026-01-22_15-06.xlsx with initial search results.
- Created S01_search_2026-01-22_15-07.xlsx with updated search results.
</commit_message>
<xml_diff>
--- a/src/P03_run_diff_sigma/T05_ml_auto_optuna/S02_combine_study.xlsx
+++ b/src/P03_run_diff_sigma/T05_ml_auto_optuna/S02_combine_study.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,21 +518,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>study_RandomForest_RS-1_TS-0_3</t>
+          <t>study_ElasticNet_RS-1_TS-0_3</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2026-01-22_14-20</t>
+          <t>2026-01-22_15-04</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>RandomForest</t>
+          <t>ElasticNet</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
@@ -542,57 +542,57 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'max_depth': 113, 'min_samples_split': 28, 'min_samples_leaf': 35, 'max_features': 0.5, 'bootstrap': False, 'criterion': 'squared_error'}</t>
+          <t>{'alpha': 0.13547865931877767, 'l1_ratio': 0.4264510492026294, 'fit_intercept': False, 'positive': False, 'max_iter': 3032, 'tol': 1.33537456273735e-06, 'selection': 'cyclic', 'warm_start': False}</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0.8046508457838573</v>
+        <v>0.8478666896436925</v>
       </c>
       <c r="I2" t="n">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="J2" t="n">
-        <v>0.8046508457838573</v>
+        <v>0.8478666896436925</v>
       </c>
       <c r="K2" t="n">
-        <v>0.02058513351683786</v>
+        <v>0.01734077905617534</v>
       </c>
       <c r="L2" t="n">
-        <v>1.440671613904355</v>
+        <v>1.60621870109394</v>
       </c>
       <c r="M2" t="n">
-        <v>0.07343277780343599</v>
+        <v>0.293769903970942</v>
       </c>
       <c r="N2" t="n">
-        <v>0.189302886208841</v>
+        <v>0.1452103068142421</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0005619527095624642</v>
+        <v>0.01293174491038636</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'max_depth': 113, 'min_samples_split': 28, 'min_samples_leaf': 35, 'max_features': 0.5, 'bootstrap': False, 'criterion': 'squared_error'}</t>
+          <t>{'alpha': 0.13547865931877767, 'l1_ratio': 0.4264510492026294, 'fit_intercept': False, 'positive': False, 'max_iter': 3032, 'tol': 1.33537456273735e-06, 'selection': 'cyclic', 'warm_start': False}</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>study_RandomForest_RS-2_TS-0_3</t>
+          <t>study_ElasticNet_RS-2_TS-0_3</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2026-01-22_14-20</t>
+          <t>2026-01-22_15-04</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>RandomForest</t>
+          <t>ElasticNet</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E3" t="n">
         <v>2</v>
@@ -602,57 +602,57 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>{'n_estimators': 75, 'max_depth': 20, 'min_samples_split': 7, 'min_samples_leaf': 20, 'max_features': 1.0, 'bootstrap': True, 'criterion': 'squared_error'}</t>
+          <t>{'alpha': 0.08511362410490068, 'l1_ratio': 0.8510132170389456, 'fit_intercept': False, 'positive': False, 'max_iter': 750, 'tol': 1.1176088259302386e-05, 'selection': 'cyclic', 'warm_start': False}</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0.8219335173840445</v>
+        <v>0.8641360919134349</v>
       </c>
       <c r="I3" t="n">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8219335173840445</v>
+        <v>0.8641360919134349</v>
       </c>
       <c r="K3" t="n">
-        <v>0.08928392115457613</v>
+        <v>0.07270429070135398</v>
       </c>
       <c r="L3" t="n">
-        <v>1.783951256459709</v>
+        <v>1.838736302121057</v>
       </c>
       <c r="M3" t="n">
-        <v>0.2709163796063078</v>
+        <v>0.3642124034894769</v>
       </c>
       <c r="N3" t="n">
-        <v>0.1744459480777718</v>
+        <v>0.1290559243513047</v>
       </c>
       <c r="O3" t="n">
-        <v>0.04116082534977507</v>
+        <v>0.02001583696189387</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>{'n_estimators': 75, 'max_depth': 20, 'min_samples_split': 7, 'min_samples_leaf': 20, 'max_features': 1.0, 'bootstrap': True, 'criterion': 'squared_error'}</t>
+          <t>{'alpha': 0.08511362410490068, 'l1_ratio': 0.8510132170389456, 'fit_intercept': False, 'positive': False, 'max_iter': 750, 'tol': 1.1176088259302386e-05, 'selection': 'cyclic', 'warm_start': False}</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>study_RandomForest_RS-3_TS-0_3</t>
+          <t>study_ElasticNet_RS-3_TS-0_3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2026-01-22_14-20</t>
+          <t>2026-01-22_15-04</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>RandomForest</t>
+          <t>ElasticNet</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E4" t="n">
         <v>3</v>
@@ -662,57 +662,57 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>{'n_estimators': 83, 'max_depth': 3, 'min_samples_split': 27, 'min_samples_leaf': 7, 'max_features': 0.8, 'bootstrap': True, 'criterion': 'squared_error'}</t>
+          <t>{'alpha': 0.23665480808740214, 'l1_ratio': 0.25344240197288337, 'fit_intercept': False, 'positive': False, 'max_iter': 6049, 'tol': 2.1733066563324934e-05, 'selection': 'random', 'warm_start': False}</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>0.8260004763952273</v>
+        <v>0.8537500551078586</v>
       </c>
       <c r="I4" t="n">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="J4" t="n">
-        <v>0.8260004763952273</v>
+        <v>0.8537500551078586</v>
       </c>
       <c r="K4" t="n">
-        <v>0.09875157866325783</v>
+        <v>0.1033286521651963</v>
       </c>
       <c r="L4" t="n">
-        <v>1.679051165007137</v>
+        <v>1.504423980895315</v>
       </c>
       <c r="M4" t="n">
-        <v>0.1793819354854832</v>
+        <v>0.09244670660909445</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1577086427453615</v>
+        <v>0.13343798769977</v>
       </c>
       <c r="O4" t="n">
-        <v>0.01504424298656838</v>
+        <v>0.00225953293790506</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>{'n_estimators': 83, 'max_depth': 3, 'min_samples_split': 27, 'min_samples_leaf': 7, 'max_features': 0.8, 'bootstrap': True, 'criterion': 'squared_error'}</t>
+          <t>{'alpha': 0.23665480808740214, 'l1_ratio': 0.25344240197288337, 'fit_intercept': False, 'positive': False, 'max_iter': 6049, 'tol': 2.1733066563324934e-05, 'selection': 'random', 'warm_start': False}</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>study_RandomForest_RS-4_TS-0_3</t>
+          <t>study_ElasticNet_RS-4_TS-0_3</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2026-01-22_14-20</t>
+          <t>2026-01-22_15-04</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>RandomForest</t>
+          <t>ElasticNet</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E5" t="n">
         <v>4</v>
@@ -722,57 +722,57 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 94, 'max_depth': 5, 'min_samples_split': 18, 'min_samples_leaf': 16, 'max_features': 1.0, 'bootstrap': True, 'criterion': 'squared_error'}</t>
+          <t>{'alpha': 0.20043967145626082, 'l1_ratio': 0.3042909555511934, 'fit_intercept': False, 'positive': False, 'max_iter': 2595, 'tol': 2.667818483311308e-06, 'selection': 'cyclic', 'warm_start': False}</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>0.8181725984996637</v>
+        <v>0.8600675446537845</v>
       </c>
       <c r="I5" t="n">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J5" t="n">
-        <v>0.8181725984996637</v>
+        <v>0.8600675446537845</v>
       </c>
       <c r="K5" t="n">
-        <v>0.04803129871993092</v>
+        <v>0.04765057380464856</v>
       </c>
       <c r="L5" t="n">
-        <v>1.821550085770723</v>
+        <v>1.729718925978498</v>
       </c>
       <c r="M5" t="n">
-        <v>0.3188925927667052</v>
+        <v>0.1632290575645513</v>
       </c>
       <c r="N5" t="n">
-        <v>0.1793191805836466</v>
+        <v>0.1375940130151955</v>
       </c>
       <c r="O5" t="n">
-        <v>0.01944258511372973</v>
+        <v>0.008345112401097121</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 94, 'max_depth': 5, 'min_samples_split': 18, 'min_samples_leaf': 16, 'max_features': 1.0, 'bootstrap': True, 'criterion': 'squared_error'}</t>
+          <t>{'alpha': 0.20043967145626082, 'l1_ratio': 0.3042909555511934, 'fit_intercept': False, 'positive': False, 'max_iter': 2595, 'tol': 2.667818483311308e-06, 'selection': 'cyclic', 'warm_start': False}</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>study_RandomForest_RS-5_TS-0_3</t>
+          <t>study_ElasticNet_RS-5_TS-0_3</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2026-01-22_14-20</t>
+          <t>2026-01-22_15-04</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>RandomForest</t>
+          <t>ElasticNet</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E6" t="n">
         <v>5</v>
@@ -782,57 +782,57 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>{'n_estimators': 95, 'max_depth': 32, 'min_samples_split': 47, 'min_samples_leaf': 6, 'max_features': 0.8, 'bootstrap': True, 'criterion': 'squared_error'}</t>
+          <t>{'alpha': 0.13547865931877767, 'l1_ratio': 0.4264510492026294, 'fit_intercept': False, 'positive': False, 'max_iter': 3032, 'tol': 1.33537456273735e-06, 'selection': 'cyclic', 'warm_start': False}</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>0.7847765880871469</v>
+        <v>0.8245488252068571</v>
       </c>
       <c r="I6" t="n">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J6" t="n">
-        <v>0.7847765880871469</v>
+        <v>0.8245488252068571</v>
       </c>
       <c r="K6" t="n">
-        <v>0.01388823372174664</v>
+        <v>0.004908903675969707</v>
       </c>
       <c r="L6" t="n">
-        <v>9.534707058695377</v>
+        <v>12.05410425866155</v>
       </c>
       <c r="M6" t="n">
-        <v>7.358936577668995</v>
+        <v>7.961051210846974</v>
       </c>
       <c r="N6" t="n">
-        <v>0.2098727180341277</v>
+        <v>0.1708117137481999</v>
       </c>
       <c r="O6" t="n">
-        <v>0.01895004215160929</v>
+        <v>0.02674864090446121</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>{'n_estimators': 95, 'max_depth': 32, 'min_samples_split': 47, 'min_samples_leaf': 6, 'max_features': 0.8, 'bootstrap': True, 'criterion': 'squared_error'}</t>
+          <t>{'alpha': 0.13547865931877767, 'l1_ratio': 0.4264510492026294, 'fit_intercept': False, 'positive': False, 'max_iter': 3032, 'tol': 1.33537456273735e-06, 'selection': 'cyclic', 'warm_start': False}</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>study_SVR_RS-1_TS-0_3</t>
+          <t>study_GradientBoosting_RS-1_TS-0_3</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2026-01-22_14-34</t>
+          <t>2026-01-22_14-48</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>SVR</t>
+          <t>GradientBoosting</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -842,57 +842,57 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>{'kernel': 'sigmoid', 'C': 61.54851719080261, 'epsilon': 1.9817013744718603e-05, 'gamma_choice': 'float', 'gamma': 4.144461934378341e-05, 'coef0': 0.23183246656516976, 'shrinking': True}</t>
+          <t>{'n_estimators': 497, 'learning_rate': 0.004547128134089966, 'max_depth': 3, 'min_samples_split': 9, 'min_samples_leaf': 9, 'subsample': 0.9723365650234614, 'max_features': 0.5, 'loss': 'absolute_error'}</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>0.9048595486405363</v>
+        <v>0.7895673956601407</v>
       </c>
       <c r="I7" t="n">
-        <v>281</v>
+        <v>60</v>
       </c>
       <c r="J7" t="n">
-        <v>0.9048595486405363</v>
+        <v>0.7895673956601407</v>
       </c>
       <c r="K7" t="n">
-        <v>0.004675800921499849</v>
+        <v>0.007461856884963772</v>
       </c>
       <c r="L7" t="n">
-        <v>1.598624612516427</v>
+        <v>1.532651143322203</v>
       </c>
       <c r="M7" t="n">
-        <v>0.2340842574520262</v>
+        <v>0.2329573099794862</v>
       </c>
       <c r="N7" t="n">
-        <v>0.08671609754694216</v>
+        <v>0.2039072463985201</v>
       </c>
       <c r="O7" t="n">
-        <v>0.02781299966982322</v>
+        <v>0.01519483355869129</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>{'kernel': 'sigmoid', 'C': 61.54851719080261, 'gamma': 4.144461934378341e-05, 'epsilon': 1.9817013744718603e-05, 'coef0': 0.23183246656516976, 'degree': 3, 'shrinking': True, 'max_iter': 1000000}</t>
+          <t>{'n_estimators': 497, 'learning_rate': 0.004547128134089966, 'max_depth': 3, 'min_samples_split': 9, 'min_samples_leaf': 9, 'subsample': 0.9723365650234614, 'max_features': 0.5, 'loss': 'absolute_error'}</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>study_SVR_RS-2_TS-0_3</t>
+          <t>study_GradientBoosting_RS-2_TS-0_3</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2026-01-22_14-34</t>
+          <t>2026-01-22_14-48</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>SVR</t>
+          <t>GradientBoosting</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E8" t="n">
         <v>2</v>
@@ -902,57 +902,57 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>{'kernel': 'sigmoid', 'C': 0.551998270742705, 'epsilon': 0.00013086876390957085, 'gamma_choice': 'auto', 'coef0': -0.24137660276488565, 'shrinking': False}</t>
+          <t>{'n_estimators': 158, 'learning_rate': 0.010229574927260657, 'max_depth': 10, 'min_samples_split': 21, 'min_samples_leaf': 29, 'subsample': 0.9954134399450667, 'max_features': 0.8, 'loss': 'squared_error'}</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>0.8852671212995747</v>
+        <v>0.8391847423255566</v>
       </c>
       <c r="I8" t="n">
-        <v>268</v>
+        <v>50</v>
       </c>
       <c r="J8" t="n">
-        <v>0.8852671212995747</v>
+        <v>0.8391847423255566</v>
       </c>
       <c r="K8" t="n">
-        <v>0.1067825094073969</v>
+        <v>0.08062905266086914</v>
       </c>
       <c r="L8" t="n">
-        <v>1.939208932155692</v>
+        <v>1.802373937365355</v>
       </c>
       <c r="M8" t="n">
-        <v>0.4837214544608053</v>
+        <v>0.2686343193519605</v>
       </c>
       <c r="N8" t="n">
-        <v>0.109646982339093</v>
+        <v>0.1554208437765472</v>
       </c>
       <c r="O8" t="n">
-        <v>0.02509245148133899</v>
+        <v>0.0278237600187774</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>{'kernel': 'sigmoid', 'C': 0.551998270742705, 'gamma': 'auto', 'epsilon': 0.00013086876390957085, 'coef0': -0.24137660276488565, 'degree': 3, 'shrinking': False, 'max_iter': 1000000}</t>
+          <t>{'n_estimators': 158, 'learning_rate': 0.010229574927260657, 'max_depth': 10, 'min_samples_split': 21, 'min_samples_leaf': 29, 'subsample': 0.9954134399450667, 'max_features': 0.8, 'loss': 'squared_error'}</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>study_SVR_RS-3_TS-0_3</t>
+          <t>study_GradientBoosting_RS-3_TS-0_3</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2026-01-22_14-34</t>
+          <t>2026-01-22_14-48</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>SVR</t>
+          <t>GradientBoosting</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E9" t="n">
         <v>3</v>
@@ -962,57 +962,57 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>{'kernel': 'sigmoid', 'C': 1.0640047554157794, 'epsilon': 0.968179596732563, 'gamma_choice': 'auto', 'coef0': -0.6354755125352025, 'shrinking': False}</t>
+          <t>{'n_estimators': 222, 'learning_rate': 0.014267664183693822, 'max_depth': 8, 'min_samples_split': 38, 'min_samples_leaf': 42, 'subsample': 0.8837076162411474, 'max_features': 0.8, 'loss': 'squared_error'}</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>0.8869095602148525</v>
+        <v>0.8278605252822183</v>
       </c>
       <c r="I9" t="n">
-        <v>262</v>
+        <v>50</v>
       </c>
       <c r="J9" t="n">
-        <v>0.8869095602148525</v>
+        <v>0.8278605252822183</v>
       </c>
       <c r="K9" t="n">
-        <v>0.1059599602819867</v>
+        <v>0.09782723652388142</v>
       </c>
       <c r="L9" t="n">
-        <v>1.467684921468336</v>
+        <v>1.583599896740913</v>
       </c>
       <c r="M9" t="n">
-        <v>0.03555978623805731</v>
+        <v>0.1084467670474062</v>
       </c>
       <c r="N9" t="n">
-        <v>0.09782734857305109</v>
+        <v>0.1573088095297857</v>
       </c>
       <c r="O9" t="n">
-        <v>0.01451759199183012</v>
+        <v>0.006280534452837523</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>{'kernel': 'sigmoid', 'C': 1.0640047554157794, 'gamma': 'auto', 'epsilon': 0.968179596732563, 'coef0': -0.6354755125352025, 'degree': 3, 'shrinking': False, 'max_iter': 1000000}</t>
+          <t>{'n_estimators': 222, 'learning_rate': 0.014267664183693822, 'max_depth': 8, 'min_samples_split': 38, 'min_samples_leaf': 42, 'subsample': 0.8837076162411474, 'max_features': 0.8, 'loss': 'squared_error'}</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>study_SVR_RS-4_TS-0_3</t>
+          <t>study_GradientBoosting_RS-4_TS-0_3</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2026-01-22_14-34</t>
+          <t>2026-01-22_14-48</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>SVR</t>
+          <t>GradientBoosting</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E10" t="n">
         <v>4</v>
@@ -1022,57 +1022,57 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>{'kernel': 'sigmoid', 'C': 0.5376231169988661, 'epsilon': 0.35143263288876353, 'gamma_choice': 'auto', 'coef0': -0.44236905692795214, 'shrinking': True}</t>
+          <t>{'n_estimators': 496, 'learning_rate': 0.0031952964444322456, 'max_depth': 2, 'min_samples_split': 15, 'min_samples_leaf': 20, 'subsample': 0.9438661569690634, 'max_features': 0.8, 'loss': 'squared_error'}</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>0.8977058842150497</v>
+        <v>0.8202594378352658</v>
       </c>
       <c r="I10" t="n">
-        <v>262</v>
+        <v>50</v>
       </c>
       <c r="J10" t="n">
-        <v>0.8977058842150497</v>
+        <v>0.8202594378352658</v>
       </c>
       <c r="K10" t="n">
-        <v>0.04700725149626973</v>
+        <v>0.05283277697401078</v>
       </c>
       <c r="L10" t="n">
-        <v>1.778908978911194</v>
+        <v>1.738378878754787</v>
       </c>
       <c r="M10" t="n">
-        <v>0.09227563561618531</v>
+        <v>0.3304735496233216</v>
       </c>
       <c r="N10" t="n">
-        <v>0.09906913443501153</v>
+        <v>0.1782742337151417</v>
       </c>
       <c r="O10" t="n">
-        <v>0.008261011783285343</v>
+        <v>0.01637493436771853</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>{'kernel': 'sigmoid', 'C': 0.5376231169988661, 'gamma': 'auto', 'epsilon': 0.35143263288876353, 'coef0': -0.44236905692795214, 'degree': 3, 'shrinking': True, 'max_iter': 1000000}</t>
+          <t>{'n_estimators': 496, 'learning_rate': 0.0031952964444322456, 'max_depth': 2, 'min_samples_split': 15, 'min_samples_leaf': 20, 'subsample': 0.9438661569690634, 'max_features': 0.8, 'loss': 'squared_error'}</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>study_SVR_RS-5_TS-0_3</t>
+          <t>study_GradientBoosting_RS-5_TS-0_3</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2026-01-22_14-34</t>
+          <t>2026-01-22_14-48</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>SVR</t>
+          <t>GradientBoosting</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E11" t="n">
         <v>5</v>
@@ -1082,34 +1082,934 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
+          <t>{'n_estimators': 166, 'learning_rate': 0.011348265086714318, 'max_depth': 9, 'min_samples_split': 58, 'min_samples_leaf': 7, 'subsample': 0.8602067346660345, 'max_features': 0.8, 'loss': 'squared_error'}</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>0.7855429452561785</v>
+      </c>
+      <c r="I11" t="n">
+        <v>50</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.7855429452561785</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.01653202017732574</v>
+      </c>
+      <c r="L11" t="n">
+        <v>11.52190982753765</v>
+      </c>
+      <c r="M11" t="n">
+        <v>10.254624691005</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.2087030257590125</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.01550475386526968</v>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 166, 'learning_rate': 0.011348265086714318, 'max_depth': 9, 'min_samples_split': 58, 'min_samples_leaf': 7, 'subsample': 0.8602067346660345, 'max_features': 0.8, 'loss': 'squared_error'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>study_KNR_RS-1_TS-0_3</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2026-01-22_15-07</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>KNR</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>50</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>{'n_neighbors': 18, 'weights': 'distance', 'algorithm': 'kd_tree', 'leaf_size': 30, 'p': 1, 'metric': 'chebyshev'}</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>0.9085420158771705</v>
+      </c>
+      <c r="I12" t="n">
+        <v>110</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.9085420158771705</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.003210303013750419</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1.447985400720352</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.1452820301195012</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.08292263469211743</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.02728414676662552</v>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>{'n_neighbors': 18, 'weights': 'distance', 'algorithm': 'kd_tree', 'leaf_size': 30, 'p': 1, 'metric': 'chebyshev'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>study_KNR_RS-2_TS-0_3</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2026-01-22_15-07</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>KNR</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>50</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>{'n_neighbors': 46, 'weights': 'distance', 'algorithm': 'ball_tree', 'leaf_size': 25, 'p': 2, 'metric': 'minkowski'}</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>0.9200324711337885</v>
+      </c>
+      <c r="I13" t="n">
+        <v>110</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.9200324711337885</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.09805978588881473</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1.548051062363585</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.2140748192932634</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.07427647424521182</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.0214318851406962</v>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>{'n_neighbors': 46, 'weights': 'distance', 'algorithm': 'ball_tree', 'leaf_size': 25, 'p': 2, 'metric': 'minkowski'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>study_KNR_RS-3_TS-0_3</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2026-01-22_15-07</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>KNR</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>50</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>{'n_neighbors': 22, 'weights': 'distance', 'algorithm': 'ball_tree', 'leaf_size': 35, 'p': 2, 'metric': 'chebyshev'}</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>0.9330085457602623</v>
+      </c>
+      <c r="I14" t="n">
+        <v>110</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.9330085457602623</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.1096047601917192</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1.40619059012438</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.08485269378711388</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.05537646300581697</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.01604411713720649</v>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>{'n_neighbors': 22, 'weights': 'distance', 'algorithm': 'ball_tree', 'leaf_size': 35, 'p': 2, 'metric': 'chebyshev'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>study_KNR_RS-4_TS-0_3</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2026-01-22_15-07</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>KNR</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>50</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>{'n_neighbors': 46, 'weights': 'distance', 'algorithm': 'auto', 'leaf_size': 32, 'p': 2, 'metric': 'minkowski'}</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>0.9101969430197369</v>
+      </c>
+      <c r="I15" t="n">
+        <v>110</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.9101969430197369</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.05384241474154881</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1.645839340140876</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.2865590550378745</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.08761983879306806</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.007597084805743513</v>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>{'n_neighbors': 46, 'weights': 'distance', 'algorithm': 'auto', 'leaf_size': 32, 'p': 2, 'metric': 'minkowski'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>study_KNR_RS-5_TS-0_3</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2026-01-22_15-07</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>KNR</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>50</v>
+      </c>
+      <c r="E16" t="n">
+        <v>5</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>{'n_neighbors': 42, 'weights': 'distance', 'algorithm': 'brute', 'leaf_size': 24, 'p': 2, 'metric': 'euclidean'}</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>0.8736559923757135</v>
+      </c>
+      <c r="I16" t="n">
+        <v>110</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.8736559923757135</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.0210510383990008</v>
+      </c>
+      <c r="L16" t="n">
+        <v>7.161875080044433</v>
+      </c>
+      <c r="M16" t="n">
+        <v>6.289297128032559</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.1213237067167424</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.008814865315342589</v>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>{'n_neighbors': 42, 'weights': 'distance', 'algorithm': 'brute', 'leaf_size': 24, 'p': 2, 'metric': 'euclidean'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>study_RandomForest_RS-1_TS-0_3</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2026-01-22_14-20</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>RandomForest</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 100, 'max_depth': 113, 'min_samples_split': 28, 'min_samples_leaf': 35, 'max_features': 0.5, 'bootstrap': False, 'criterion': 'squared_error'}</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>0.8046508457838573</v>
+      </c>
+      <c r="I17" t="n">
+        <v>119</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.8046508457838573</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.02058513351683786</v>
+      </c>
+      <c r="L17" t="n">
+        <v>1.440671613904355</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.07343277780343599</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.189302886208841</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.0005619527095624642</v>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 100, 'max_depth': 113, 'min_samples_split': 28, 'min_samples_leaf': 35, 'max_features': 0.5, 'bootstrap': False, 'criterion': 'squared_error'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>study_RandomForest_RS-2_TS-0_3</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2026-01-22_14-20</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>RandomForest</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 75, 'max_depth': 20, 'min_samples_split': 7, 'min_samples_leaf': 20, 'max_features': 1.0, 'bootstrap': True, 'criterion': 'squared_error'}</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>0.8219335173840445</v>
+      </c>
+      <c r="I18" t="n">
+        <v>119</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.8219335173840445</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.08928392115457613</v>
+      </c>
+      <c r="L18" t="n">
+        <v>1.783951256459709</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.2709163796063078</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.1744459480777718</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.04116082534977507</v>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 75, 'max_depth': 20, 'min_samples_split': 7, 'min_samples_leaf': 20, 'max_features': 1.0, 'bootstrap': True, 'criterion': 'squared_error'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>study_RandomForest_RS-3_TS-0_3</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2026-01-22_14-20</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>RandomForest</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 83, 'max_depth': 3, 'min_samples_split': 27, 'min_samples_leaf': 7, 'max_features': 0.8, 'bootstrap': True, 'criterion': 'squared_error'}</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>0.8260004763952273</v>
+      </c>
+      <c r="I19" t="n">
+        <v>123</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.8260004763952273</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.09875157866325783</v>
+      </c>
+      <c r="L19" t="n">
+        <v>1.679051165007137</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.1793819354854832</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.1577086427453615</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.01504424298656838</v>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 83, 'max_depth': 3, 'min_samples_split': 27, 'min_samples_leaf': 7, 'max_features': 0.8, 'bootstrap': True, 'criterion': 'squared_error'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>study_RandomForest_RS-4_TS-0_3</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2026-01-22_14-20</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>RandomForest</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>4</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 94, 'max_depth': 5, 'min_samples_split': 18, 'min_samples_leaf': 16, 'max_features': 1.0, 'bootstrap': True, 'criterion': 'squared_error'}</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>0.8181725984996637</v>
+      </c>
+      <c r="I20" t="n">
+        <v>113</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.8181725984996637</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.04803129871993092</v>
+      </c>
+      <c r="L20" t="n">
+        <v>1.821550085770723</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.3188925927667052</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.1793191805836466</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.01944258511372973</v>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 94, 'max_depth': 5, 'min_samples_split': 18, 'min_samples_leaf': 16, 'max_features': 1.0, 'bootstrap': True, 'criterion': 'squared_error'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>study_RandomForest_RS-5_TS-0_3</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2026-01-22_14-20</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>RandomForest</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>5</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 95, 'max_depth': 32, 'min_samples_split': 47, 'min_samples_leaf': 6, 'max_features': 0.8, 'bootstrap': True, 'criterion': 'squared_error'}</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>0.7847765880871469</v>
+      </c>
+      <c r="I21" t="n">
+        <v>113</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.7847765880871469</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.01388823372174664</v>
+      </c>
+      <c r="L21" t="n">
+        <v>9.534707058695377</v>
+      </c>
+      <c r="M21" t="n">
+        <v>7.358936577668995</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.2098727180341277</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.01895004215160929</v>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 95, 'max_depth': 32, 'min_samples_split': 47, 'min_samples_leaf': 6, 'max_features': 0.8, 'bootstrap': True, 'criterion': 'squared_error'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>study_SVR_RS-1_TS-0_3</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2026-01-22_14-34</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>SVR</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>100</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>{'kernel': 'sigmoid', 'C': 61.54851719080261, 'epsilon': 1.9817013744718603e-05, 'gamma_choice': 'float', 'gamma': 4.144461934378341e-05, 'coef0': 0.23183246656516976, 'shrinking': True}</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>0.9048595486405363</v>
+      </c>
+      <c r="I22" t="n">
+        <v>281</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.9048595486405363</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.004675800921499849</v>
+      </c>
+      <c r="L22" t="n">
+        <v>1.598624612516427</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.2340842574520262</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.08671609754694216</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.02781299966982322</v>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>{'kernel': 'sigmoid', 'C': 61.54851719080261, 'gamma': 4.144461934378341e-05, 'epsilon': 1.9817013744718603e-05, 'coef0': 0.23183246656516976, 'degree': 3, 'shrinking': True, 'max_iter': 1000000}</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>study_SVR_RS-2_TS-0_3</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2026-01-22_14-34</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>SVR</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>100</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>{'kernel': 'sigmoid', 'C': 0.551998270742705, 'epsilon': 0.00013086876390957085, 'gamma_choice': 'auto', 'coef0': -0.24137660276488565, 'shrinking': False}</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>0.8852671212995747</v>
+      </c>
+      <c r="I23" t="n">
+        <v>268</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.8852671212995747</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.1067825094073969</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1.939208932155692</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.4837214544608053</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.109646982339093</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.02509245148133899</v>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>{'kernel': 'sigmoid', 'C': 0.551998270742705, 'gamma': 'auto', 'epsilon': 0.00013086876390957085, 'coef0': -0.24137660276488565, 'degree': 3, 'shrinking': False, 'max_iter': 1000000}</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>study_SVR_RS-3_TS-0_3</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2026-01-22_14-34</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>SVR</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>100</v>
+      </c>
+      <c r="E24" t="n">
+        <v>3</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>{'kernel': 'sigmoid', 'C': 1.0640047554157794, 'epsilon': 0.968179596732563, 'gamma_choice': 'auto', 'coef0': -0.6354755125352025, 'shrinking': False}</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>0.8869095602148525</v>
+      </c>
+      <c r="I24" t="n">
+        <v>262</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.8869095602148525</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.1059599602819867</v>
+      </c>
+      <c r="L24" t="n">
+        <v>1.467684921468336</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.03555978623805731</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.09782734857305109</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.01451759199183012</v>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>{'kernel': 'sigmoid', 'C': 1.0640047554157794, 'gamma': 'auto', 'epsilon': 0.968179596732563, 'coef0': -0.6354755125352025, 'degree': 3, 'shrinking': False, 'max_iter': 1000000}</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>study_SVR_RS-4_TS-0_3</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2026-01-22_14-34</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>SVR</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>100</v>
+      </c>
+      <c r="E25" t="n">
+        <v>4</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>{'kernel': 'sigmoid', 'C': 0.5376231169988661, 'epsilon': 0.35143263288876353, 'gamma_choice': 'auto', 'coef0': -0.44236905692795214, 'shrinking': True}</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>0.8977058842150497</v>
+      </c>
+      <c r="I25" t="n">
+        <v>262</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.8977058842150497</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.04700725149626973</v>
+      </c>
+      <c r="L25" t="n">
+        <v>1.778908978911194</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.09227563561618531</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.09906913443501153</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0.008261011783285343</v>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>{'kernel': 'sigmoid', 'C': 0.5376231169988661, 'gamma': 'auto', 'epsilon': 0.35143263288876353, 'coef0': -0.44236905692795214, 'degree': 3, 'shrinking': True, 'max_iter': 1000000}</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>study_SVR_RS-5_TS-0_3</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2026-01-22_14-34</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>SVR</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>100</v>
+      </c>
+      <c r="E26" t="n">
+        <v>5</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>{'kernel': 'poly', 'C': 0.13061121247736907, 'epsilon': 2.5590511016126443e-06, 'gamma_choice': 'scale', 'coef0': 0.9983333243743104, 'degree': 2, 'shrinking': False}</t>
         </is>
       </c>
-      <c r="H11" t="n">
+      <c r="H26" t="n">
         <v>0.887515515518334</v>
       </c>
-      <c r="I11" t="n">
+      <c r="I26" t="n">
         <v>262</v>
       </c>
-      <c r="J11" t="n">
+      <c r="J26" t="n">
         <v>0.887515515518334</v>
       </c>
-      <c r="K11" t="n">
+      <c r="K26" t="n">
         <v>0.04666763037134115</v>
       </c>
-      <c r="L11" t="n">
+      <c r="L26" t="n">
         <v>6.511720268191776</v>
       </c>
-      <c r="M11" t="n">
+      <c r="M26" t="n">
         <v>5.221458663135831</v>
       </c>
-      <c r="N11" t="n">
+      <c r="N26" t="n">
         <v>0.1055685980132071</v>
       </c>
-      <c r="O11" t="n">
+      <c r="O26" t="n">
         <v>0.02632745075778458</v>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="P26" t="inlineStr">
         <is>
           <t>{'kernel': 'poly', 'C': 0.13061121247736907, 'gamma': 'scale', 'epsilon': 2.5590511016126443e-06, 'coef0': 0.9983333243743104, 'degree': 2, 'shrinking': False, 'max_iter': 1000000}</t>
         </is>

</xml_diff>